<commit_message>
finished reviewing scraped data
</commit_message>
<xml_diff>
--- a/data/update2019/ospree_2019update_my.xlsx
+++ b/data/update2019/ospree_2019update_my.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/ospree/data/update2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9DBFF0-157D-0A4F-AE98-4972BA9B6F65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068D4896-C237-894B-9562-7487A8794182}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="16260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="16420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,19 @@
     <sheet name="data_detailed" sheetId="1" r:id="rId4"/>
     <sheet name="scratch" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -81,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="346">
   <si>
     <t>datasetID</t>
   </si>
@@ -1002,45 +1008,18 @@
     <t>no</t>
   </si>
   <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>12/01/2017</t>
-  </si>
-  <si>
-    <t>02/11/2016</t>
-  </si>
-  <si>
-    <t>daystobudburst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ambient </t>
-  </si>
-  <si>
-    <t>maleflower-cuttings</t>
-  </si>
-  <si>
-    <t>femaleflower-cuttings</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>SE</t>
   </si>
   <si>
-    <t>table1, table2</t>
-  </si>
-  <si>
     <t>4, 9, 4.4, 5.7, 4.3</t>
   </si>
   <si>
     <t>90days</t>
   </si>
   <si>
-    <t>16, 5.7, 14.4, 4.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Webster Nursery, south of Olympia, Washington </t>
   </si>
   <si>
@@ -1086,24 +1065,6 @@
     <t>avium</t>
   </si>
   <si>
-    <t>27/02/2014</t>
-  </si>
-  <si>
-    <t>05/04/2014</t>
-  </si>
-  <si>
-    <t>01/05/2014</t>
-  </si>
-  <si>
-    <t>17/05/2014</t>
-  </si>
-  <si>
-    <t>30/05/2014</t>
-  </si>
-  <si>
-    <t>29/01/2014</t>
-  </si>
-  <si>
     <t>thermaltimetobudburst</t>
   </si>
   <si>
@@ -1129,16 +1090,53 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>daystoflowering</t>
+  </si>
+  <si>
+    <t>ambientgreenhouse_4.4</t>
+  </si>
+  <si>
+    <t>ambientgreenhouse_4.5</t>
+  </si>
+  <si>
+    <t>ambient_5.7</t>
+  </si>
+  <si>
+    <t>webstergreenhouse_4.3</t>
+  </si>
+  <si>
+    <t>webstergreenhouse_4.4</t>
+  </si>
+  <si>
+    <t>webster_4.5</t>
+  </si>
+  <si>
+    <t>webster_4.6</t>
+  </si>
+  <si>
+    <t>table 2</t>
+  </si>
+  <si>
+    <t>16, ambient5.7_webstergreenhouse14.4_webster4.3</t>
+  </si>
+  <si>
+    <t>webstergreenhouse_14.4</t>
+  </si>
+  <si>
+    <t>webster_4.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1218,6 +1216,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1251,7 +1255,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1295,6 +1299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1406,7 +1411,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1458,7 +1463,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3043,12 +3048,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
@@ -3126,25 +3134,25 @@
         <v>296</v>
       </c>
       <c r="F2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G2" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="H2" t="s">
         <v>304</v>
       </c>
       <c r="M2" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="O2" t="s">
         <v>304</v>
       </c>
       <c r="S2" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="T2" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -3155,31 +3163,31 @@
         <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="E3" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="F3" t="s">
         <v>304</v>
       </c>
       <c r="J3" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="O3" t="s">
         <v>304</v>
       </c>
       <c r="S3" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="T3" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3196,17 +3204,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AB42" sqref="AB42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="63" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" customWidth="1"/>
     <col min="11" max="11" width="20.5" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" customWidth="1"/>
     <col min="22" max="23" width="12.6640625" customWidth="1"/>
+    <col min="31" max="31" width="22" customWidth="1"/>
     <col min="34" max="34" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3409,13 +3420,13 @@
         <v>2016</v>
       </c>
       <c r="O2" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="P2" t="s">
         <v>305</v>
       </c>
-      <c r="Q2" t="s">
-        <v>308</v>
+      <c r="Q2" s="21">
+        <v>42675</v>
       </c>
       <c r="R2">
         <v>4</v>
@@ -3439,7 +3450,7 @@
         <v>304</v>
       </c>
       <c r="Y2" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z2">
         <v>1</v>
@@ -3451,22 +3462,16 @@
         <v>9</v>
       </c>
       <c r="AC2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD2">
         <v>1.4</v>
       </c>
       <c r="AE2" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF2">
-        <v>46.952244</v>
-      </c>
-      <c r="AG2">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:53">
@@ -3507,13 +3512,13 @@
         <v>2016</v>
       </c>
       <c r="O3" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="P3" t="s">
         <v>305</v>
       </c>
-      <c r="Q3" t="s">
-        <v>308</v>
+      <c r="Q3" s="21">
+        <v>42675</v>
       </c>
       <c r="R3">
         <v>4</v>
@@ -3537,7 +3542,7 @@
         <v>304</v>
       </c>
       <c r="Y3" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z3">
         <v>1</v>
@@ -3549,22 +3554,16 @@
         <v>7</v>
       </c>
       <c r="AC3" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD3">
         <v>1.6</v>
       </c>
       <c r="AE3" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF3">
-        <v>46.952244</v>
-      </c>
-      <c r="AG3">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH3" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:53">
@@ -3605,13 +3604,13 @@
         <v>2016</v>
       </c>
       <c r="O4" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="P4" t="s">
         <v>305</v>
       </c>
-      <c r="Q4" t="s">
-        <v>308</v>
+      <c r="Q4" s="21">
+        <v>42675</v>
       </c>
       <c r="R4">
         <v>9</v>
@@ -3635,7 +3634,7 @@
         <v>304</v>
       </c>
       <c r="Y4" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z4">
         <v>1</v>
@@ -3647,22 +3646,16 @@
         <v>4</v>
       </c>
       <c r="AC4" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD4">
         <v>2.2999999999999998</v>
       </c>
       <c r="AE4" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF4">
-        <v>46.952244</v>
-      </c>
-      <c r="AG4">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH4" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:53">
@@ -3703,13 +3696,13 @@
         <v>2016</v>
       </c>
       <c r="O5" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="P5" t="s">
         <v>305</v>
       </c>
-      <c r="Q5" t="s">
-        <v>308</v>
+      <c r="Q5" s="21">
+        <v>42675</v>
       </c>
       <c r="R5">
         <v>9</v>
@@ -3733,7 +3726,7 @@
         <v>304</v>
       </c>
       <c r="Y5" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z5">
         <v>1</v>
@@ -3745,22 +3738,16 @@
         <v>4</v>
       </c>
       <c r="AC5" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD5">
         <v>6.3</v>
       </c>
       <c r="AE5" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF5">
-        <v>46.952244</v>
-      </c>
-      <c r="AG5">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH5" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:53">
@@ -3801,16 +3788,16 @@
         <v>2016</v>
       </c>
       <c r="O6" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="P6" t="s">
         <v>305</v>
       </c>
-      <c r="Q6" t="s">
-        <v>308</v>
-      </c>
-      <c r="R6">
-        <v>4.4000000000000004</v>
+      <c r="Q6" s="21">
+        <v>42675</v>
+      </c>
+      <c r="R6" t="s">
+        <v>335</v>
       </c>
       <c r="S6" t="s">
         <v>304</v>
@@ -3831,7 +3818,7 @@
         <v>304</v>
       </c>
       <c r="Y6" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z6">
         <v>1</v>
@@ -3843,22 +3830,16 @@
         <v>5</v>
       </c>
       <c r="AC6" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD6">
         <v>3.2</v>
       </c>
       <c r="AE6" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF6">
-        <v>46.952244</v>
-      </c>
-      <c r="AG6">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:53">
@@ -3899,16 +3880,16 @@
         <v>2016</v>
       </c>
       <c r="O7" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="P7" t="s">
         <v>305</v>
       </c>
-      <c r="Q7" t="s">
-        <v>308</v>
-      </c>
-      <c r="R7">
-        <v>4.4000000000000004</v>
+      <c r="Q7" s="21">
+        <v>42675</v>
+      </c>
+      <c r="R7" t="s">
+        <v>336</v>
       </c>
       <c r="S7" t="s">
         <v>304</v>
@@ -3929,28 +3910,25 @@
         <v>304</v>
       </c>
       <c r="Y7" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z7">
         <v>1</v>
       </c>
       <c r="AA7" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="AB7">
         <v>0</v>
       </c>
+      <c r="AD7" t="s">
+        <v>306</v>
+      </c>
       <c r="AE7" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF7">
-        <v>46.952244</v>
-      </c>
-      <c r="AG7">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH7" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:53">
@@ -3991,25 +3969,22 @@
         <v>2016</v>
       </c>
       <c r="O8" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="P8" t="s">
         <v>305</v>
       </c>
-      <c r="Q8" t="s">
-        <v>308</v>
-      </c>
-      <c r="R8">
-        <v>5.7</v>
+      <c r="Q8" s="21">
+        <v>42675</v>
+      </c>
+      <c r="R8" t="s">
+        <v>337</v>
       </c>
       <c r="S8" t="s">
         <v>304</v>
       </c>
-      <c r="T8" t="s">
-        <v>310</v>
-      </c>
-      <c r="U8">
-        <v>5.7</v>
+      <c r="U8" t="s">
+        <v>337</v>
       </c>
       <c r="V8">
         <v>5.7</v>
@@ -4021,7 +3996,7 @@
         <v>304</v>
       </c>
       <c r="Y8" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z8">
         <v>1</v>
@@ -4033,22 +4008,16 @@
         <v>4</v>
       </c>
       <c r="AC8" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD8">
         <v>2.7</v>
       </c>
       <c r="AE8" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF8">
-        <v>46.952244</v>
-      </c>
-      <c r="AG8">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH8" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:53">
@@ -4089,25 +4058,22 @@
         <v>2016</v>
       </c>
       <c r="O9" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="P9" t="s">
         <v>305</v>
       </c>
-      <c r="Q9" t="s">
-        <v>308</v>
-      </c>
-      <c r="R9">
-        <v>5.7</v>
+      <c r="Q9" s="21">
+        <v>42675</v>
+      </c>
+      <c r="R9" t="s">
+        <v>337</v>
       </c>
       <c r="S9" t="s">
         <v>304</v>
       </c>
-      <c r="T9" t="s">
-        <v>304</v>
-      </c>
-      <c r="U9">
-        <v>5.7</v>
+      <c r="U9" t="s">
+        <v>337</v>
       </c>
       <c r="V9">
         <v>5.7</v>
@@ -4119,7 +4085,7 @@
         <v>304</v>
       </c>
       <c r="Y9" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z9">
         <v>1</v>
@@ -4131,22 +4097,16 @@
         <v>4</v>
       </c>
       <c r="AC9" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD9">
         <v>3.1</v>
       </c>
       <c r="AE9" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF9">
-        <v>46.952244</v>
-      </c>
-      <c r="AG9">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH9" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:53">
@@ -4187,16 +4147,16 @@
         <v>2017</v>
       </c>
       <c r="O10" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="P10" t="s">
         <v>299</v>
       </c>
-      <c r="Q10" t="s">
-        <v>307</v>
-      </c>
-      <c r="R10">
-        <v>4.3</v>
+      <c r="Q10" s="21">
+        <v>42747</v>
+      </c>
+      <c r="R10" t="s">
+        <v>338</v>
       </c>
       <c r="S10" t="s">
         <v>304</v>
@@ -4204,8 +4164,8 @@
       <c r="T10">
         <v>90</v>
       </c>
-      <c r="U10">
-        <v>14.4</v>
+      <c r="U10" t="s">
+        <v>344</v>
       </c>
       <c r="V10">
         <v>14.4</v>
@@ -4217,7 +4177,7 @@
         <v>304</v>
       </c>
       <c r="Y10" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z10">
         <v>1</v>
@@ -4229,22 +4189,16 @@
         <v>9</v>
       </c>
       <c r="AC10" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD10">
         <v>4.2</v>
       </c>
       <c r="AE10" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF10">
-        <v>38.898555999999999</v>
-      </c>
-      <c r="AG10">
-        <v>-77.037852000000001</v>
+        <v>342</v>
       </c>
       <c r="AH10" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:53">
@@ -4285,16 +4239,16 @@
         <v>2017</v>
       </c>
       <c r="O11" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="P11" t="s">
         <v>299</v>
       </c>
-      <c r="Q11" t="s">
-        <v>307</v>
-      </c>
-      <c r="R11">
-        <v>4.3</v>
+      <c r="Q11" s="21">
+        <v>42747</v>
+      </c>
+      <c r="R11" t="s">
+        <v>339</v>
       </c>
       <c r="S11" t="s">
         <v>304</v>
@@ -4302,8 +4256,8 @@
       <c r="T11">
         <v>90</v>
       </c>
-      <c r="U11">
-        <v>14.4</v>
+      <c r="U11" t="s">
+        <v>344</v>
       </c>
       <c r="V11">
         <v>14.4</v>
@@ -4315,7 +4269,7 @@
         <v>304</v>
       </c>
       <c r="Y11" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z11">
         <v>1</v>
@@ -4327,22 +4281,16 @@
         <v>9</v>
       </c>
       <c r="AC11" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD11">
         <v>0.9</v>
       </c>
       <c r="AE11" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF11">
-        <v>38.898555999999999</v>
-      </c>
-      <c r="AG11">
-        <v>-77.037852000000001</v>
+        <v>342</v>
       </c>
       <c r="AH11" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:53">
@@ -4383,25 +4331,22 @@
         <v>2017</v>
       </c>
       <c r="O12" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="P12" t="s">
         <v>299</v>
       </c>
-      <c r="Q12" t="s">
-        <v>307</v>
-      </c>
-      <c r="R12">
-        <v>4.3</v>
+      <c r="Q12" s="21">
+        <v>42747</v>
+      </c>
+      <c r="R12" t="s">
+        <v>340</v>
       </c>
       <c r="S12" t="s">
         <v>304</v>
       </c>
-      <c r="T12" t="s">
-        <v>306</v>
-      </c>
-      <c r="U12">
-        <v>4.3</v>
+      <c r="U12" t="s">
+        <v>345</v>
       </c>
       <c r="V12">
         <v>4.3</v>
@@ -4413,7 +4358,7 @@
         <v>304</v>
       </c>
       <c r="Y12" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z12">
         <v>1</v>
@@ -4425,22 +4370,16 @@
         <v>6</v>
       </c>
       <c r="AC12" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD12">
         <v>2</v>
       </c>
       <c r="AE12" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF12">
-        <v>46.952244</v>
-      </c>
-      <c r="AG12">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH12" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:53">
@@ -4481,25 +4420,22 @@
         <v>2017</v>
       </c>
       <c r="O13" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="P13" t="s">
         <v>299</v>
       </c>
-      <c r="Q13" t="s">
-        <v>307</v>
-      </c>
-      <c r="R13">
-        <v>4.3</v>
+      <c r="Q13" s="21">
+        <v>42747</v>
+      </c>
+      <c r="R13" t="s">
+        <v>341</v>
       </c>
       <c r="S13" t="s">
         <v>304</v>
       </c>
-      <c r="T13" t="s">
-        <v>306</v>
-      </c>
-      <c r="U13">
-        <v>4.3</v>
+      <c r="U13" t="s">
+        <v>345</v>
       </c>
       <c r="V13">
         <v>4.3</v>
@@ -4511,7 +4447,7 @@
         <v>304</v>
       </c>
       <c r="Y13" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -4523,22 +4459,16 @@
         <v>4</v>
       </c>
       <c r="AC13" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AD13">
         <v>5</v>
       </c>
       <c r="AE13" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF13">
-        <v>46.952244</v>
-      </c>
-      <c r="AG13">
-        <v>-122.959158</v>
+        <v>342</v>
       </c>
       <c r="AH13" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:53">
@@ -4549,22 +4479,22 @@
         <v>303</v>
       </c>
       <c r="C14" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D14" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="E14" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G14" t="s">
         <v>299</v>
       </c>
       <c r="H14" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I14" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J14">
         <v>47.47</v>
@@ -4573,10 +4503,10 @@
         <v>7.5</v>
       </c>
       <c r="L14" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M14" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N14">
         <v>2014</v>
@@ -4587,8 +4517,8 @@
       <c r="P14" t="s">
         <v>299</v>
       </c>
-      <c r="Q14" t="s">
-        <v>334</v>
+      <c r="Q14" s="21">
+        <v>41697</v>
       </c>
       <c r="S14" t="s">
         <v>304</v>
@@ -4603,7 +4533,7 @@
         <v>304</v>
       </c>
       <c r="Y14" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA14">
         <v>528.86599999999999</v>
@@ -4612,13 +4542,13 @@
         <v>5</v>
       </c>
       <c r="AC14" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD14">
         <v>45</v>
       </c>
       <c r="AE14" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:53">
@@ -4629,22 +4559,22 @@
         <v>303</v>
       </c>
       <c r="C15" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="E15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G15" t="s">
         <v>299</v>
       </c>
       <c r="H15" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I15" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J15">
         <v>47.47</v>
@@ -4653,10 +4583,10 @@
         <v>7.5</v>
       </c>
       <c r="L15" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M15" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N15">
         <v>2014</v>
@@ -4667,8 +4597,8 @@
       <c r="P15" t="s">
         <v>299</v>
       </c>
-      <c r="Q15" t="s">
-        <v>335</v>
+      <c r="Q15" s="21">
+        <v>42099</v>
       </c>
       <c r="S15" t="s">
         <v>304</v>
@@ -4683,7 +4613,7 @@
         <v>304</v>
       </c>
       <c r="Y15" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA15">
         <v>190.72200000000001</v>
@@ -4692,13 +4622,13 @@
         <v>5</v>
       </c>
       <c r="AC15" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD15">
         <v>22</v>
       </c>
       <c r="AE15" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:53">
@@ -4709,22 +4639,22 @@
         <v>303</v>
       </c>
       <c r="C16" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D16" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="E16" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G16" t="s">
         <v>299</v>
       </c>
       <c r="H16" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I16" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J16">
         <v>47.47</v>
@@ -4733,10 +4663,10 @@
         <v>7.5</v>
       </c>
       <c r="L16" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M16" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N16">
         <v>2014</v>
@@ -4747,8 +4677,8 @@
       <c r="P16" t="s">
         <v>299</v>
       </c>
-      <c r="Q16" t="s">
-        <v>336</v>
+      <c r="Q16" s="21">
+        <v>41760</v>
       </c>
       <c r="S16" t="s">
         <v>304</v>
@@ -4763,7 +4693,7 @@
         <v>304</v>
       </c>
       <c r="Y16" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA16">
         <v>50.515000000000001</v>
@@ -4772,13 +4702,13 @@
         <v>5</v>
       </c>
       <c r="AC16" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD16">
         <v>24</v>
       </c>
       <c r="AE16" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -4789,22 +4719,22 @@
         <v>303</v>
       </c>
       <c r="C17" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="E17" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G17" t="s">
         <v>299</v>
       </c>
       <c r="H17" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I17" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J17">
         <v>47.47</v>
@@ -4813,10 +4743,10 @@
         <v>7.5</v>
       </c>
       <c r="L17" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M17" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N17">
         <v>2014</v>
@@ -4827,8 +4757,8 @@
       <c r="P17" t="s">
         <v>299</v>
       </c>
-      <c r="Q17" t="s">
-        <v>337</v>
+      <c r="Q17" s="21">
+        <v>41776</v>
       </c>
       <c r="S17" t="s">
         <v>304</v>
@@ -4843,7 +4773,7 @@
         <v>304</v>
       </c>
       <c r="Y17" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA17">
         <v>0</v>
@@ -4852,10 +4782,10 @@
         <v>5</v>
       </c>
       <c r="AC17" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE17" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -4866,22 +4796,22 @@
         <v>303</v>
       </c>
       <c r="C18" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D18" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="E18" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G18" t="s">
         <v>299</v>
       </c>
       <c r="H18" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I18" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J18">
         <v>47.47</v>
@@ -4890,10 +4820,10 @@
         <v>7.5</v>
       </c>
       <c r="L18" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M18" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N18">
         <v>2014</v>
@@ -4904,8 +4834,8 @@
       <c r="P18" t="s">
         <v>299</v>
       </c>
-      <c r="Q18" t="s">
-        <v>338</v>
+      <c r="Q18" s="21">
+        <v>41789</v>
       </c>
       <c r="S18" t="s">
         <v>304</v>
@@ -4920,7 +4850,7 @@
         <v>304</v>
       </c>
       <c r="Y18" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA18">
         <v>0</v>
@@ -4929,10 +4859,10 @@
         <v>5</v>
       </c>
       <c r="AC18" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE18" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:31">
@@ -4943,22 +4873,22 @@
         <v>303</v>
       </c>
       <c r="C19" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D19" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E19" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="G19" t="s">
         <v>299</v>
       </c>
       <c r="H19" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I19" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J19">
         <v>47.47</v>
@@ -4967,10 +4897,10 @@
         <v>7.5</v>
       </c>
       <c r="L19" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M19" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N19">
         <v>2014</v>
@@ -4981,8 +4911,8 @@
       <c r="P19" t="s">
         <v>299</v>
       </c>
-      <c r="Q19" t="s">
-        <v>339</v>
+      <c r="Q19" s="21">
+        <v>41668</v>
       </c>
       <c r="S19" t="s">
         <v>304</v>
@@ -4997,7 +4927,7 @@
         <v>304</v>
       </c>
       <c r="Y19" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA19">
         <v>243.077</v>
@@ -5006,13 +4936,13 @@
         <v>5</v>
       </c>
       <c r="AC19" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD19">
         <v>26</v>
       </c>
       <c r="AE19" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -5023,22 +4953,22 @@
         <v>303</v>
       </c>
       <c r="C20" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D20" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E20" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="G20" t="s">
         <v>299</v>
       </c>
       <c r="H20" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I20" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J20">
         <v>47.47</v>
@@ -5047,10 +4977,10 @@
         <v>7.5</v>
       </c>
       <c r="L20" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M20" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N20">
         <v>2014</v>
@@ -5061,8 +4991,8 @@
       <c r="P20" t="s">
         <v>299</v>
       </c>
-      <c r="Q20" t="s">
-        <v>334</v>
+      <c r="Q20" s="21">
+        <v>41697</v>
       </c>
       <c r="S20" t="s">
         <v>304</v>
@@ -5077,7 +5007,7 @@
         <v>304</v>
       </c>
       <c r="Y20" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA20">
         <v>126.154</v>
@@ -5086,13 +5016,13 @@
         <v>5</v>
       </c>
       <c r="AC20" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD20">
         <v>26</v>
       </c>
       <c r="AE20" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:31">
@@ -5103,22 +5033,22 @@
         <v>303</v>
       </c>
       <c r="C21" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D21" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E21" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="G21" t="s">
         <v>299</v>
       </c>
       <c r="H21" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I21" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J21">
         <v>47.47</v>
@@ -5127,10 +5057,10 @@
         <v>7.5</v>
       </c>
       <c r="L21" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M21" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N21">
         <v>2014</v>
@@ -5141,8 +5071,8 @@
       <c r="P21" t="s">
         <v>299</v>
       </c>
-      <c r="Q21" t="s">
-        <v>335</v>
+      <c r="Q21" s="21">
+        <v>42099</v>
       </c>
       <c r="S21" t="s">
         <v>304</v>
@@ -5157,7 +5087,7 @@
         <v>304</v>
       </c>
       <c r="Y21" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA21">
         <v>0</v>
@@ -5166,10 +5096,10 @@
         <v>5</v>
       </c>
       <c r="AC21" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE21" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:31">
@@ -5180,22 +5110,22 @@
         <v>303</v>
       </c>
       <c r="C22" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D22" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E22" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="G22" t="s">
         <v>299</v>
       </c>
       <c r="H22" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I22" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J22">
         <v>47.47</v>
@@ -5204,10 +5134,10 @@
         <v>7.5</v>
       </c>
       <c r="L22" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M22" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N22">
         <v>2014</v>
@@ -5218,8 +5148,8 @@
       <c r="P22" t="s">
         <v>299</v>
       </c>
-      <c r="Q22" t="s">
-        <v>336</v>
+      <c r="Q22" s="21">
+        <v>41760</v>
       </c>
       <c r="S22" t="s">
         <v>304</v>
@@ -5234,7 +5164,7 @@
         <v>304</v>
       </c>
       <c r="Y22" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA22">
         <v>0</v>
@@ -5243,10 +5173,10 @@
         <v>5</v>
       </c>
       <c r="AC22" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE22" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -5257,22 +5187,22 @@
         <v>303</v>
       </c>
       <c r="C23" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D23" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E23" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="G23" t="s">
         <v>299</v>
       </c>
       <c r="H23" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I23" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J23">
         <v>47.47</v>
@@ -5281,10 +5211,10 @@
         <v>7.5</v>
       </c>
       <c r="L23" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M23" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N23">
         <v>2014</v>
@@ -5295,8 +5225,8 @@
       <c r="P23" t="s">
         <v>299</v>
       </c>
-      <c r="Q23" t="s">
-        <v>337</v>
+      <c r="Q23" s="21">
+        <v>41776</v>
       </c>
       <c r="S23" t="s">
         <v>304</v>
@@ -5311,7 +5241,7 @@
         <v>304</v>
       </c>
       <c r="Y23" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -5320,10 +5250,10 @@
         <v>5</v>
       </c>
       <c r="AC23" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE23" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -5334,22 +5264,22 @@
         <v>303</v>
       </c>
       <c r="C24" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D24" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E24" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G24" t="s">
         <v>299</v>
       </c>
       <c r="H24" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I24" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J24">
         <v>47.47</v>
@@ -5358,10 +5288,10 @@
         <v>7.5</v>
       </c>
       <c r="L24" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M24" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N24">
         <v>2014</v>
@@ -5372,8 +5302,8 @@
       <c r="P24" t="s">
         <v>299</v>
       </c>
-      <c r="Q24" t="s">
-        <v>339</v>
+      <c r="Q24" s="21">
+        <v>41668</v>
       </c>
       <c r="S24" t="s">
         <v>304</v>
@@ -5388,7 +5318,7 @@
         <v>304</v>
       </c>
       <c r="Y24" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA24">
         <v>390.74599999999998</v>
@@ -5397,10 +5327,10 @@
         <v>5</v>
       </c>
       <c r="AC24" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE24" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -5411,22 +5341,22 @@
         <v>303</v>
       </c>
       <c r="C25" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D25" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E25" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G25" t="s">
         <v>299</v>
       </c>
       <c r="H25" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I25" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J25">
         <v>47.47</v>
@@ -5435,10 +5365,10 @@
         <v>7.5</v>
       </c>
       <c r="L25" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M25" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N25">
         <v>2014</v>
@@ -5449,8 +5379,8 @@
       <c r="P25" t="s">
         <v>299</v>
       </c>
-      <c r="Q25" t="s">
-        <v>334</v>
+      <c r="Q25" s="21">
+        <v>41697</v>
       </c>
       <c r="S25" t="s">
         <v>304</v>
@@ -5465,7 +5395,7 @@
         <v>304</v>
       </c>
       <c r="Y25" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA25">
         <v>332.13400000000001</v>
@@ -5474,10 +5404,10 @@
         <v>5</v>
       </c>
       <c r="AC25" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE25" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:31">
@@ -5488,22 +5418,22 @@
         <v>303</v>
       </c>
       <c r="C26" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D26" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E26" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G26" t="s">
         <v>299</v>
       </c>
       <c r="H26" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I26" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J26">
         <v>47.47</v>
@@ -5512,10 +5442,10 @@
         <v>7.5</v>
       </c>
       <c r="L26" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M26" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N26">
         <v>2014</v>
@@ -5526,8 +5456,8 @@
       <c r="P26" t="s">
         <v>299</v>
       </c>
-      <c r="Q26" t="s">
-        <v>335</v>
+      <c r="Q26" s="21">
+        <v>42099</v>
       </c>
       <c r="S26" t="s">
         <v>304</v>
@@ -5542,7 +5472,7 @@
         <v>304</v>
       </c>
       <c r="Y26" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA26">
         <v>177.892</v>
@@ -5551,10 +5481,10 @@
         <v>5</v>
       </c>
       <c r="AC26" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE26" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -5565,22 +5495,22 @@
         <v>303</v>
       </c>
       <c r="C27" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D27" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E27" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G27" t="s">
         <v>299</v>
       </c>
       <c r="H27" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I27" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J27">
         <v>47.47</v>
@@ -5589,10 +5519,10 @@
         <v>7.5</v>
       </c>
       <c r="L27" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M27" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N27">
         <v>2014</v>
@@ -5603,8 +5533,8 @@
       <c r="P27" t="s">
         <v>299</v>
       </c>
-      <c r="Q27" t="s">
-        <v>336</v>
+      <c r="Q27" s="21">
+        <v>41760</v>
       </c>
       <c r="S27" t="s">
         <v>304</v>
@@ -5619,7 +5549,7 @@
         <v>304</v>
       </c>
       <c r="Y27" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA27">
         <v>47.301000000000002</v>
@@ -5628,10 +5558,10 @@
         <v>5</v>
       </c>
       <c r="AC27" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE27" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:31">
@@ -5642,22 +5572,22 @@
         <v>303</v>
       </c>
       <c r="C28" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D28" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E28" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G28" t="s">
         <v>299</v>
       </c>
       <c r="H28" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I28" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J28">
         <v>47.47</v>
@@ -5666,10 +5596,10 @@
         <v>7.5</v>
       </c>
       <c r="L28" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M28" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N28">
         <v>2014</v>
@@ -5680,8 +5610,8 @@
       <c r="P28" t="s">
         <v>299</v>
       </c>
-      <c r="Q28" t="s">
-        <v>337</v>
+      <c r="Q28" s="21">
+        <v>41776</v>
       </c>
       <c r="S28" t="s">
         <v>304</v>
@@ -5696,7 +5626,7 @@
         <v>304</v>
       </c>
       <c r="Y28" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA28">
         <v>0</v>
@@ -5705,10 +5635,10 @@
         <v>5</v>
       </c>
       <c r="AC28" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE28" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:31">
@@ -5719,22 +5649,22 @@
         <v>303</v>
       </c>
       <c r="C29" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D29" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E29" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G29" t="s">
         <v>299</v>
       </c>
       <c r="H29" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I29" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J29">
         <v>47.47</v>
@@ -5743,10 +5673,10 @@
         <v>7.5</v>
       </c>
       <c r="L29" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M29" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N29">
         <v>2014</v>
@@ -5757,8 +5687,8 @@
       <c r="P29" t="s">
         <v>299</v>
       </c>
-      <c r="Q29" t="s">
-        <v>338</v>
+      <c r="Q29" s="21">
+        <v>41789</v>
       </c>
       <c r="S29" t="s">
         <v>304</v>
@@ -5773,7 +5703,7 @@
         <v>304</v>
       </c>
       <c r="Y29" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -5782,10 +5712,10 @@
         <v>5</v>
       </c>
       <c r="AC29" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE29" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:31">
@@ -5796,22 +5726,22 @@
         <v>303</v>
       </c>
       <c r="C30" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D30" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E30" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G30" t="s">
         <v>299</v>
       </c>
       <c r="H30" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I30" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J30">
         <v>47.47</v>
@@ -5820,10 +5750,10 @@
         <v>7.5</v>
       </c>
       <c r="L30" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M30" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N30">
         <v>2014</v>
@@ -5834,8 +5764,8 @@
       <c r="P30" t="s">
         <v>299</v>
       </c>
-      <c r="Q30" t="s">
-        <v>339</v>
+      <c r="Q30" s="21">
+        <v>41668</v>
       </c>
       <c r="S30" t="s">
         <v>304</v>
@@ -5850,7 +5780,7 @@
         <v>304</v>
       </c>
       <c r="Y30" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA30">
         <v>321.851</v>
@@ -5859,13 +5789,13 @@
         <v>4</v>
       </c>
       <c r="AC30" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD30">
         <v>33</v>
       </c>
       <c r="AE30" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="1:31">
@@ -5876,22 +5806,22 @@
         <v>303</v>
       </c>
       <c r="C31" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D31" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E31" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G31" t="s">
         <v>299</v>
       </c>
       <c r="H31" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I31" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J31">
         <v>47.47</v>
@@ -5900,10 +5830,10 @@
         <v>7.5</v>
       </c>
       <c r="L31" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M31" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N31">
         <v>2014</v>
@@ -5914,8 +5844,8 @@
       <c r="P31" t="s">
         <v>299</v>
       </c>
-      <c r="Q31" t="s">
-        <v>334</v>
+      <c r="Q31" s="21">
+        <v>41697</v>
       </c>
       <c r="S31" t="s">
         <v>304</v>
@@ -5930,7 +5860,7 @@
         <v>304</v>
       </c>
       <c r="Y31" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA31">
         <v>183.03299999999999</v>
@@ -5939,13 +5869,13 @@
         <v>4</v>
       </c>
       <c r="AC31" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD31">
         <v>30</v>
       </c>
       <c r="AE31" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" spans="1:31">
@@ -5956,22 +5886,22 @@
         <v>303</v>
       </c>
       <c r="C32" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D32" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E32" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G32" t="s">
         <v>299</v>
       </c>
       <c r="H32" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I32" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J32">
         <v>47.47</v>
@@ -5980,10 +5910,10 @@
         <v>7.5</v>
       </c>
       <c r="L32" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M32" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N32">
         <v>2014</v>
@@ -5994,8 +5924,8 @@
       <c r="P32" t="s">
         <v>299</v>
       </c>
-      <c r="Q32" t="s">
-        <v>335</v>
+      <c r="Q32" s="21">
+        <v>42099</v>
       </c>
       <c r="S32" t="s">
         <v>304</v>
@@ -6010,7 +5940,7 @@
         <v>304</v>
       </c>
       <c r="Y32" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA32">
         <v>58.612000000000002</v>
@@ -6019,13 +5949,13 @@
         <v>4</v>
       </c>
       <c r="AC32" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AD32">
         <v>32</v>
       </c>
       <c r="AE32" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:31">
@@ -6036,22 +5966,22 @@
         <v>303</v>
       </c>
       <c r="C33" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D33" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E33" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G33" t="s">
         <v>299</v>
       </c>
       <c r="H33" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I33" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J33">
         <v>47.47</v>
@@ -6060,10 +5990,10 @@
         <v>7.5</v>
       </c>
       <c r="L33" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M33" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N33">
         <v>2014</v>
@@ -6074,8 +6004,8 @@
       <c r="P33" t="s">
         <v>299</v>
       </c>
-      <c r="Q33" t="s">
-        <v>336</v>
+      <c r="Q33" s="21">
+        <v>41760</v>
       </c>
       <c r="S33" t="s">
         <v>304</v>
@@ -6090,7 +6020,7 @@
         <v>304</v>
       </c>
       <c r="Y33" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA33">
         <v>0</v>
@@ -6099,10 +6029,10 @@
         <v>4</v>
       </c>
       <c r="AC33" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE33" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:31">
@@ -6113,22 +6043,22 @@
         <v>303</v>
       </c>
       <c r="C34" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D34" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E34" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G34" t="s">
         <v>299</v>
       </c>
       <c r="H34" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I34" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J34">
         <v>47.47</v>
@@ -6137,10 +6067,10 @@
         <v>7.5</v>
       </c>
       <c r="L34" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M34" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N34">
         <v>2014</v>
@@ -6151,8 +6081,8 @@
       <c r="P34" t="s">
         <v>299</v>
       </c>
-      <c r="Q34" t="s">
-        <v>337</v>
+      <c r="Q34" s="21">
+        <v>41776</v>
       </c>
       <c r="S34" t="s">
         <v>304</v>
@@ -6167,19 +6097,19 @@
         <v>304</v>
       </c>
       <c r="Y34" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA34" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="AB34">
         <v>4</v>
       </c>
       <c r="AC34" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE34" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="35" spans="1:31">
@@ -6190,22 +6120,22 @@
         <v>303</v>
       </c>
       <c r="C35" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D35" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E35" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G35" t="s">
         <v>299</v>
       </c>
       <c r="H35" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I35" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J35">
         <v>47.47</v>
@@ -6214,10 +6144,10 @@
         <v>7.5</v>
       </c>
       <c r="L35" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="M35" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="N35">
         <v>2014</v>
@@ -6228,8 +6158,8 @@
       <c r="P35" t="s">
         <v>299</v>
       </c>
-      <c r="Q35" t="s">
-        <v>338</v>
+      <c r="Q35" s="21">
+        <v>41789</v>
       </c>
       <c r="S35" t="s">
         <v>304</v>
@@ -6244,22 +6174,23 @@
         <v>304</v>
       </c>
       <c r="Y35" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AA35" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="AB35">
         <v>4</v>
       </c>
       <c r="AC35" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AE35" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
updating prevey and ramos
</commit_message>
<xml_diff>
--- a/data/update2019/ospree_2019update_my.xlsx
+++ b/data/update2019/ospree_2019update_my.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/ospree/data/update2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/ospree/data/update2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068D4896-C237-894B-9562-7487A8794182}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494C206C-E7F1-2E4B-92E0-0E11C376D4B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="16420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="460" windowWidth="28780" windowHeight="16420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="343">
   <si>
     <t>datasetID</t>
   </si>
@@ -1005,9 +1005,6 @@
     <t>ambient</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -1095,24 +1092,6 @@
     <t>daystoflowering</t>
   </si>
   <si>
-    <t>ambientgreenhouse_4.4</t>
-  </si>
-  <si>
-    <t>ambientgreenhouse_4.5</t>
-  </si>
-  <si>
-    <t>ambient_5.7</t>
-  </si>
-  <si>
-    <t>webstergreenhouse_4.3</t>
-  </si>
-  <si>
-    <t>webstergreenhouse_4.4</t>
-  </si>
-  <si>
-    <t>webster_4.5</t>
-  </si>
-  <si>
     <t>webster_4.6</t>
   </si>
   <si>
@@ -1122,10 +1101,22 @@
     <t>16, ambient5.7_webstergreenhouse14.4_webster4.3</t>
   </si>
   <si>
-    <t>webstergreenhouse_14.4</t>
-  </si>
-  <si>
     <t>webster_4.3</t>
+  </si>
+  <si>
+    <t>cjc</t>
+  </si>
+  <si>
+    <t>Alnus</t>
+  </si>
+  <si>
+    <t>daystoflower</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
+  </si>
+  <si>
+    <t>supp</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1127,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1255,7 +1246,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1290,6 +1281,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1299,7 +1291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1671,19 +1663,19 @@
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="60.5" customWidth="1"/>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34">
+    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17">
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>274</v>
       </c>
@@ -1694,7 +1686,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17">
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1702,7 +1694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17">
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>126</v>
       </c>
@@ -1720,7 +1712,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:16" ht="17">
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>127</v>
       </c>
@@ -1728,7 +1720,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="17">
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>128</v>
       </c>
@@ -1736,7 +1728,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="17">
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>129</v>
       </c>
@@ -1744,7 +1736,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17">
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>130</v>
       </c>
@@ -1752,7 +1744,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="17">
+    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>131</v>
       </c>
@@ -1760,7 +1752,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="17">
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>132</v>
       </c>
@@ -1768,7 +1760,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="17">
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>134</v>
       </c>
@@ -1776,7 +1768,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="17">
+    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>135</v>
       </c>
@@ -1784,7 +1776,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="17">
+    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>136</v>
       </c>
@@ -1792,7 +1784,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>137</v>
       </c>
@@ -1800,7 +1792,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>138</v>
       </c>
@@ -1808,7 +1800,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>139</v>
       </c>
@@ -1819,7 +1811,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>174</v>
       </c>
@@ -1828,7 +1820,7 @@
       </c>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
@@ -1837,7 +1829,7 @@
       </c>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>177</v>
       </c>
@@ -1846,7 +1838,7 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="17">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>140</v>
       </c>
@@ -1854,7 +1846,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>141</v>
       </c>
@@ -1862,7 +1854,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>142</v>
       </c>
@@ -1870,12 +1862,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17">
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>275</v>
       </c>
@@ -1883,11 +1875,11 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="17">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1887,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17">
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>144</v>
       </c>
@@ -1903,7 +1895,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>145</v>
       </c>
@@ -1911,7 +1903,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>146</v>
       </c>
@@ -1919,7 +1911,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17">
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>103</v>
       </c>
@@ -1927,7 +1919,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>147</v>
       </c>
@@ -1935,7 +1927,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>148</v>
       </c>
@@ -1943,7 +1935,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17">
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>149</v>
       </c>
@@ -1951,7 +1943,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17">
+    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>150</v>
       </c>
@@ -1959,7 +1951,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>151</v>
       </c>
@@ -1967,7 +1959,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="34">
+    <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>152</v>
       </c>
@@ -1975,7 +1967,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17">
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>153</v>
       </c>
@@ -1983,7 +1975,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17">
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>154</v>
       </c>
@@ -1991,7 +1983,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>155</v>
       </c>
@@ -1999,7 +1991,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17">
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>156</v>
       </c>
@@ -2007,7 +1999,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17">
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>157</v>
       </c>
@@ -2015,7 +2007,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17">
+    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>158</v>
       </c>
@@ -2023,7 +2015,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17">
+    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>159</v>
       </c>
@@ -2031,7 +2023,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17">
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2039,7 +2031,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17">
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>136</v>
       </c>
@@ -2047,7 +2039,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17">
+    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>276</v>
       </c>
@@ -2055,7 +2047,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17">
+    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2055,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17">
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>1</v>
       </c>
@@ -2071,7 +2063,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17">
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
@@ -2079,7 +2071,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17">
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
@@ -2087,7 +2079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17">
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
@@ -2095,7 +2087,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17">
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2095,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17">
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
@@ -2111,7 +2103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17">
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -2119,7 +2111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17">
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>61</v>
       </c>
@@ -2133,7 +2125,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17">
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>64</v>
       </c>
@@ -2141,7 +2133,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="17">
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>67</v>
       </c>
@@ -2149,7 +2141,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="17">
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>12</v>
       </c>
@@ -2157,7 +2149,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="17">
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>13</v>
       </c>
@@ -2165,7 +2157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17">
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>14</v>
       </c>
@@ -2173,7 +2165,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17">
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>15</v>
       </c>
@@ -2181,7 +2173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17">
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>72</v>
       </c>
@@ -2189,7 +2181,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17">
+    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>17</v>
       </c>
@@ -2197,7 +2189,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="17">
+    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>18</v>
       </c>
@@ -2205,7 +2197,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17">
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>19</v>
       </c>
@@ -2213,7 +2205,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="17">
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>20</v>
       </c>
@@ -2221,7 +2213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="17">
+    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>21</v>
       </c>
@@ -2229,7 +2221,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17">
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
@@ -2237,7 +2229,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="17">
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>23</v>
       </c>
@@ -2245,7 +2237,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="17">
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>24</v>
       </c>
@@ -2253,27 +2245,27 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="17">
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B79" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="17">
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="18"/>
-    </row>
-    <row r="81" spans="1:3" ht="17">
+      <c r="C80" s="19"/>
+    </row>
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>27</v>
       </c>
@@ -2281,7 +2273,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="17">
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
@@ -2289,7 +2281,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="17">
+    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>29</v>
       </c>
@@ -2297,7 +2289,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="17">
+    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>90</v>
       </c>
@@ -2305,37 +2297,37 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="17">
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B85" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C85" s="19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="17">
+    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B86" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="18"/>
-    </row>
-    <row r="87" spans="1:3" ht="17">
+      <c r="C86" s="19"/>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="17">
+    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17">
+    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>99</v>
       </c>
@@ -2343,7 +2335,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="17">
+    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>101</v>
       </c>
@@ -2351,7 +2343,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="17">
+    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>103</v>
       </c>
@@ -2359,7 +2351,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="17">
+    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>36</v>
       </c>
@@ -2367,7 +2359,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="17">
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>106</v>
       </c>
@@ -2375,7 +2367,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="17">
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>38</v>
       </c>
@@ -2383,102 +2375,102 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="17">
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="17">
+    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B96" t="s">
         <v>110</v>
       </c>
-      <c r="C96" s="18" t="s">
+      <c r="C96" s="19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17">
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B97" t="s">
         <v>112</v>
       </c>
-      <c r="C97" s="20"/>
-    </row>
-    <row r="98" spans="1:3" ht="34">
+      <c r="C97" s="21"/>
+    </row>
+    <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B98" t="s">
         <v>113</v>
       </c>
-      <c r="C98" s="20"/>
-    </row>
-    <row r="99" spans="1:3" ht="34">
+      <c r="C98" s="21"/>
+    </row>
+    <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B99" t="s">
         <v>114</v>
       </c>
-      <c r="C99" s="20"/>
-    </row>
-    <row r="100" spans="1:3" ht="17">
+      <c r="C99" s="21"/>
+    </row>
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B100" t="s">
         <v>116</v>
       </c>
-      <c r="C100" s="18" t="s">
+      <c r="C100" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="34">
+    <row r="101" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B101" t="s">
         <v>119</v>
       </c>
-      <c r="C101" s="18"/>
-    </row>
-    <row r="102" spans="1:3" ht="34">
+      <c r="C101" s="19"/>
+    </row>
+    <row r="102" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B102" t="s">
         <v>121</v>
       </c>
-      <c r="C102" s="18"/>
-    </row>
-    <row r="103" spans="1:3" ht="17">
+      <c r="C102" s="19"/>
+    </row>
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B103" t="s">
         <v>123</v>
       </c>
-      <c r="C103" s="18"/>
-    </row>
-    <row r="104" spans="1:3" ht="34">
+      <c r="C103" s="19"/>
+    </row>
+    <row r="104" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B104" t="s">
         <v>125</v>
       </c>
-      <c r="C104" s="18"/>
-    </row>
-    <row r="106" spans="1:3" ht="17">
+      <c r="C104" s="19"/>
+    </row>
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
         <v>282</v>
       </c>
@@ -2486,7 +2478,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
         <v>283</v>
       </c>
@@ -2494,7 +2486,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
         <v>284</v>
       </c>
@@ -2502,7 +2494,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="9" t="s">
         <v>285</v>
       </c>
@@ -2510,7 +2502,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
         <v>286</v>
       </c>
@@ -2518,7 +2510,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
         <v>287</v>
       </c>
@@ -2526,55 +2518,55 @@
         <v>293</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="10"/>
       <c r="B113" s="11"/>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="10"/>
       <c r="B114" s="11"/>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="11"/>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="10"/>
       <c r="B116" s="11"/>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="19"/>
-      <c r="B117" s="19"/>
-    </row>
-    <row r="118" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="20"/>
+      <c r="B117" s="20"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="10"/>
       <c r="B119" s="11"/>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="10"/>
       <c r="B120" s="11"/>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="10"/>
       <c r="B121" s="11"/>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="10"/>
       <c r="B122" s="11"/>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="10"/>
       <c r="B123" s="11"/>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="10"/>
       <c r="B124" s="11"/>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
     </row>
@@ -2617,13 +2609,13 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1">
+    <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2682,7 +2674,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -2711,7 +2703,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -2737,7 +2729,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>211</v>
       </c>
@@ -2766,7 +2758,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -2795,7 +2787,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>213</v>
       </c>
@@ -2819,7 +2811,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>214</v>
       </c>
@@ -2848,7 +2840,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -2877,7 +2869,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>216</v>
       </c>
@@ -2906,7 +2898,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>217</v>
       </c>
@@ -2935,7 +2927,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>218</v>
       </c>
@@ -2964,7 +2956,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>219</v>
       </c>
@@ -2993,7 +2985,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -3053,12 +3045,12 @@
       <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="13" max="13" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3120,7 +3112,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -3134,28 +3126,28 @@
         <v>296</v>
       </c>
       <c r="F2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G2" t="s">
         <v>308</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>304</v>
+      </c>
+      <c r="M2" t="s">
+        <v>336</v>
+      </c>
+      <c r="O2" t="s">
+        <v>304</v>
+      </c>
+      <c r="S2" t="s">
         <v>309</v>
       </c>
-      <c r="H2" t="s">
-        <v>304</v>
-      </c>
-      <c r="M2" t="s">
-        <v>343</v>
-      </c>
-      <c r="O2" t="s">
-        <v>304</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>310</v>
       </c>
-      <c r="T2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -3163,31 +3155,31 @@
         <v>303</v>
       </c>
       <c r="C3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D3" t="s">
         <v>327</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>328</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" t="s">
         <v>329</v>
       </c>
-      <c r="F3" t="s">
-        <v>304</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="O3" t="s">
+        <v>304</v>
+      </c>
+      <c r="S3" t="s">
+        <v>318</v>
+      </c>
+      <c r="T3" t="s">
         <v>331</v>
-      </c>
-      <c r="O3" t="s">
-        <v>304</v>
-      </c>
-      <c r="S3" t="s">
-        <v>319</v>
-      </c>
-      <c r="T3" t="s">
-        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3204,11 +3196,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="63" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="63" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
@@ -3221,7 +3213,7 @@
     <col min="34" max="34" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="1" customFormat="1">
+    <row r="1" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3382,18 +3374,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:53">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>213</v>
       </c>
       <c r="B2" t="s">
         <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E2" t="s">
         <v>298</v>
@@ -3423,9 +3415,9 @@
         <v>296</v>
       </c>
       <c r="P2" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q2" s="21">
+        <v>299</v>
+      </c>
+      <c r="Q2" s="22">
         <v>42675</v>
       </c>
       <c r="R2">
@@ -3450,42 +3442,42 @@
         <v>304</v>
       </c>
       <c r="Y2" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z2">
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>44.8</v>
+        <v>46.857142857142897</v>
       </c>
       <c r="AB2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC2" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD2">
-        <v>1.4</v>
+        <v>4.25944329025016</v>
       </c>
       <c r="AE2" t="s">
         <v>342</v>
       </c>
       <c r="AH2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53">
-      <c r="A3" s="9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>213</v>
       </c>
       <c r="B3" t="s">
         <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E3" t="s">
         <v>298</v>
@@ -3515,9 +3507,9 @@
         <v>296</v>
       </c>
       <c r="P3" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q3" s="21">
+        <v>299</v>
+      </c>
+      <c r="Q3" s="22">
         <v>42675</v>
       </c>
       <c r="R3">
@@ -3542,31 +3534,31 @@
         <v>304</v>
       </c>
       <c r="Y3" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AA3">
-        <v>46.9</v>
+        <v>44.7777777777778</v>
       </c>
       <c r="AB3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AC3" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD3">
-        <v>1.6</v>
+        <v>4.2064764880413197</v>
       </c>
       <c r="AE3" t="s">
         <v>342</v>
       </c>
       <c r="AH3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -3574,10 +3566,10 @@
         <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D4" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E4" t="s">
         <v>298</v>
@@ -3607,9 +3599,9 @@
         <v>296</v>
       </c>
       <c r="P4" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q4" s="21">
+        <v>299</v>
+      </c>
+      <c r="Q4" s="22">
         <v>42675</v>
       </c>
       <c r="R4">
@@ -3634,31 +3626,31 @@
         <v>304</v>
       </c>
       <c r="Y4" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z4">
         <v>1</v>
       </c>
       <c r="AA4">
-        <v>55.7</v>
+        <v>57.3333333333333</v>
       </c>
       <c r="AB4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC4" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD4">
-        <v>2.2999999999999998</v>
+        <v>4.0414518843273797</v>
       </c>
       <c r="AE4" t="s">
         <v>342</v>
       </c>
       <c r="AH4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -3666,10 +3658,10 @@
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E5" t="s">
         <v>298</v>
@@ -3699,9 +3691,9 @@
         <v>296</v>
       </c>
       <c r="P5" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q5" s="21">
+        <v>299</v>
+      </c>
+      <c r="Q5" s="22">
         <v>42675</v>
       </c>
       <c r="R5">
@@ -3726,31 +3718,31 @@
         <v>304</v>
       </c>
       <c r="Y5" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z5">
         <v>1</v>
       </c>
       <c r="AA5">
-        <v>57.3</v>
+        <v>55.6666666666667</v>
       </c>
       <c r="AB5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC5" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD5">
-        <v>6.3</v>
+        <v>10.969655114602901</v>
       </c>
       <c r="AE5" t="s">
         <v>342</v>
       </c>
       <c r="AH5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>213</v>
       </c>
@@ -3758,10 +3750,10 @@
         <v>303</v>
       </c>
       <c r="C6" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D6" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E6" t="s">
         <v>298</v>
@@ -3791,25 +3783,22 @@
         <v>296</v>
       </c>
       <c r="P6" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q6" s="21">
+        <v>299</v>
+      </c>
+      <c r="Q6" s="22">
         <v>42675</v>
       </c>
       <c r="R6" t="s">
-        <v>335</v>
+        <v>304</v>
       </c>
       <c r="S6" t="s">
         <v>304</v>
       </c>
-      <c r="T6">
-        <v>90</v>
-      </c>
-      <c r="U6">
-        <v>16</v>
-      </c>
-      <c r="V6">
-        <v>16</v>
+      <c r="U6" t="s">
+        <v>304</v>
+      </c>
+      <c r="V6" t="s">
+        <v>304</v>
       </c>
       <c r="W6" t="s">
         <v>304</v>
@@ -3818,31 +3807,31 @@
         <v>304</v>
       </c>
       <c r="Y6" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z6">
         <v>1</v>
       </c>
       <c r="AA6">
-        <v>64.5</v>
+        <v>65.454545454545496</v>
       </c>
       <c r="AB6">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="AC6" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD6">
-        <v>3.2</v>
+        <v>12.5089059182939</v>
       </c>
       <c r="AE6" t="s">
         <v>342</v>
       </c>
       <c r="AH6" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>213</v>
       </c>
@@ -3850,10 +3839,10 @@
         <v>303</v>
       </c>
       <c r="C7" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E7" t="s">
         <v>298</v>
@@ -3883,13 +3872,13 @@
         <v>296</v>
       </c>
       <c r="P7" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q7" s="21">
-        <v>42675</v>
+        <v>299</v>
+      </c>
+      <c r="Q7" s="22">
+        <v>42766</v>
       </c>
       <c r="R7" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="S7" t="s">
         <v>304</v>
@@ -3910,28 +3899,31 @@
         <v>304</v>
       </c>
       <c r="Y7" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z7">
         <v>1</v>
       </c>
-      <c r="AA7" t="s">
-        <v>306</v>
+      <c r="AA7">
+        <v>53.5</v>
       </c>
       <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>306</v>
+        <v>4</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>341</v>
+      </c>
+      <c r="AD7">
+        <v>5.4467115461227298</v>
       </c>
       <c r="AE7" t="s">
         <v>342</v>
       </c>
       <c r="AH7" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -3939,10 +3931,10 @@
         <v>303</v>
       </c>
       <c r="C8" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D8" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E8" t="s">
         <v>298</v>
@@ -3972,22 +3964,25 @@
         <v>296</v>
       </c>
       <c r="P8" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q8" s="21">
-        <v>42675</v>
+        <v>299</v>
+      </c>
+      <c r="Q8" s="22">
+        <v>42766</v>
       </c>
       <c r="R8" t="s">
-        <v>337</v>
+        <v>304</v>
       </c>
       <c r="S8" t="s">
         <v>304</v>
       </c>
-      <c r="U8" t="s">
-        <v>337</v>
+      <c r="T8">
+        <v>90</v>
+      </c>
+      <c r="U8">
+        <v>16</v>
       </c>
       <c r="V8">
-        <v>5.7</v>
+        <v>16</v>
       </c>
       <c r="W8" t="s">
         <v>304</v>
@@ -3996,31 +3991,31 @@
         <v>304</v>
       </c>
       <c r="Y8" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z8">
         <v>1</v>
       </c>
       <c r="AA8">
-        <v>53.2</v>
+        <v>53.1666666666667</v>
       </c>
       <c r="AB8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC8" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD8">
-        <v>2.7</v>
+        <v>7.6789756261279196</v>
       </c>
       <c r="AE8" t="s">
         <v>342</v>
       </c>
       <c r="AH8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -4028,10 +4023,10 @@
         <v>303</v>
       </c>
       <c r="C9" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E9" t="s">
         <v>298</v>
@@ -4061,22 +4056,22 @@
         <v>296</v>
       </c>
       <c r="P9" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q9" s="21">
+        <v>299</v>
+      </c>
+      <c r="Q9" s="22">
         <v>42675</v>
       </c>
       <c r="R9" t="s">
-        <v>337</v>
+        <v>304</v>
       </c>
       <c r="S9" t="s">
         <v>304</v>
       </c>
       <c r="U9" t="s">
-        <v>337</v>
-      </c>
-      <c r="V9">
-        <v>5.7</v>
+        <v>304</v>
+      </c>
+      <c r="V9" t="s">
+        <v>304</v>
       </c>
       <c r="W9" t="s">
         <v>304</v>
@@ -4085,31 +4080,31 @@
         <v>304</v>
       </c>
       <c r="Y9" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z9">
         <v>1</v>
       </c>
       <c r="AA9">
-        <v>53.5</v>
+        <v>67.3333333333333</v>
       </c>
       <c r="AB9">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AC9" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD9">
-        <v>3.1</v>
+        <v>1.3228756555323</v>
       </c>
       <c r="AE9" t="s">
         <v>342</v>
       </c>
       <c r="AH9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>213</v>
       </c>
@@ -4117,10 +4112,10 @@
         <v>303</v>
       </c>
       <c r="C10" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D10" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E10" t="s">
         <v>298</v>
@@ -4144,7 +4139,7 @@
         <v>302</v>
       </c>
       <c r="N10">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="O10" t="s">
         <v>296</v>
@@ -4152,23 +4147,20 @@
       <c r="P10" t="s">
         <v>299</v>
       </c>
-      <c r="Q10" s="21">
-        <v>42747</v>
+      <c r="Q10" s="22">
+        <v>42675</v>
       </c>
       <c r="R10" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
       <c r="S10" t="s">
         <v>304</v>
       </c>
-      <c r="T10">
-        <v>90</v>
-      </c>
       <c r="U10" t="s">
-        <v>344</v>
-      </c>
-      <c r="V10">
-        <v>14.4</v>
+        <v>304</v>
+      </c>
+      <c r="V10" t="s">
+        <v>304</v>
       </c>
       <c r="W10" t="s">
         <v>304</v>
@@ -4177,31 +4169,31 @@
         <v>304</v>
       </c>
       <c r="Y10" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z10">
         <v>1</v>
       </c>
       <c r="AA10">
-        <v>67.5</v>
+        <v>72.1111111111111</v>
       </c>
       <c r="AB10">
         <v>9</v>
       </c>
       <c r="AC10" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD10">
-        <v>4.2</v>
+        <v>2.9767618499152899</v>
       </c>
       <c r="AE10" t="s">
         <v>342</v>
       </c>
       <c r="AH10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>213</v>
       </c>
@@ -4209,10 +4201,10 @@
         <v>303</v>
       </c>
       <c r="C11" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D11" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E11" t="s">
         <v>298</v>
@@ -4236,7 +4228,7 @@
         <v>302</v>
       </c>
       <c r="N11">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="O11" t="s">
         <v>296</v>
@@ -4244,11 +4236,11 @@
       <c r="P11" t="s">
         <v>299</v>
       </c>
-      <c r="Q11" s="21">
-        <v>42747</v>
+      <c r="Q11" s="22">
+        <v>42766</v>
       </c>
       <c r="R11" t="s">
-        <v>339</v>
+        <v>304</v>
       </c>
       <c r="S11" t="s">
         <v>304</v>
@@ -4256,8 +4248,8 @@
       <c r="T11">
         <v>90</v>
       </c>
-      <c r="U11" t="s">
-        <v>344</v>
+      <c r="U11">
+        <v>14.4</v>
       </c>
       <c r="V11">
         <v>14.4</v>
@@ -4269,31 +4261,31 @@
         <v>304</v>
       </c>
       <c r="Y11" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="Z11">
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>72.8</v>
+        <v>45.5</v>
       </c>
       <c r="AB11">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="AC11" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD11">
-        <v>0.9</v>
+        <v>3</v>
       </c>
       <c r="AE11" t="s">
         <v>342</v>
       </c>
       <c r="AH11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -4301,10 +4293,10 @@
         <v>303</v>
       </c>
       <c r="C12" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="E12" t="s">
         <v>298</v>
@@ -4328,7 +4320,7 @@
         <v>302</v>
       </c>
       <c r="N12">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="O12" t="s">
         <v>296</v>
@@ -4336,29 +4328,32 @@
       <c r="P12" t="s">
         <v>299</v>
       </c>
-      <c r="Q12" s="21">
-        <v>42747</v>
+      <c r="Q12" s="22">
+        <v>42766</v>
       </c>
       <c r="R12" t="s">
+        <v>304</v>
+      </c>
+      <c r="S12" t="s">
+        <v>304</v>
+      </c>
+      <c r="T12">
+        <v>90</v>
+      </c>
+      <c r="U12">
+        <v>14.4</v>
+      </c>
+      <c r="V12">
+        <v>14.4</v>
+      </c>
+      <c r="W12" t="s">
+        <v>304</v>
+      </c>
+      <c r="X12" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y12" t="s">
         <v>340</v>
-      </c>
-      <c r="S12" t="s">
-        <v>304</v>
-      </c>
-      <c r="U12" t="s">
-        <v>345</v>
-      </c>
-      <c r="V12">
-        <v>4.3</v>
-      </c>
-      <c r="W12" t="s">
-        <v>304</v>
-      </c>
-      <c r="X12" t="s">
-        <v>304</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>334</v>
       </c>
       <c r="Z12">
         <v>1</v>
@@ -4370,19 +4365,19 @@
         <v>6</v>
       </c>
       <c r="AC12" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="AD12">
-        <v>2</v>
+        <v>5.0199601592044498</v>
       </c>
       <c r="AE12" t="s">
         <v>342</v>
       </c>
       <c r="AH12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="13" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>213</v>
       </c>
@@ -4425,17 +4420,17 @@
       <c r="P13" t="s">
         <v>299</v>
       </c>
-      <c r="Q13" s="21">
-        <v>42747</v>
+      <c r="Q13" s="22">
+        <v>42766</v>
       </c>
       <c r="R13" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="S13" t="s">
         <v>304</v>
       </c>
       <c r="U13" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="V13">
         <v>4.3</v>
@@ -4447,7 +4442,7 @@
         <v>304</v>
       </c>
       <c r="Y13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -4459,19 +4454,19 @@
         <v>4</v>
       </c>
       <c r="AC13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AD13">
         <v>5</v>
       </c>
       <c r="AE13" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="AH13" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>212</v>
       </c>
@@ -4479,22 +4474,22 @@
         <v>303</v>
       </c>
       <c r="C14" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
         <v>312</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>313</v>
       </c>
-      <c r="E14" t="s">
-        <v>314</v>
-      </c>
       <c r="G14" t="s">
         <v>299</v>
       </c>
       <c r="H14" t="s">
+        <v>318</v>
+      </c>
+      <c r="I14" t="s">
         <v>319</v>
-      </c>
-      <c r="I14" t="s">
-        <v>320</v>
       </c>
       <c r="J14">
         <v>47.47</v>
@@ -4503,10 +4498,10 @@
         <v>7.5</v>
       </c>
       <c r="L14" t="s">
+        <v>320</v>
+      </c>
+      <c r="M14" t="s">
         <v>321</v>
-      </c>
-      <c r="M14" t="s">
-        <v>322</v>
       </c>
       <c r="N14">
         <v>2014</v>
@@ -4517,7 +4512,7 @@
       <c r="P14" t="s">
         <v>299</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="18">
         <v>41697</v>
       </c>
       <c r="S14" t="s">
@@ -4533,7 +4528,7 @@
         <v>304</v>
       </c>
       <c r="Y14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA14">
         <v>528.86599999999999</v>
@@ -4542,16 +4537,16 @@
         <v>5</v>
       </c>
       <c r="AC14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD14">
         <v>45</v>
       </c>
       <c r="AE14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>212</v>
       </c>
@@ -4559,22 +4554,22 @@
         <v>303</v>
       </c>
       <c r="C15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
         <v>312</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>313</v>
       </c>
-      <c r="E15" t="s">
-        <v>314</v>
-      </c>
       <c r="G15" t="s">
         <v>299</v>
       </c>
       <c r="H15" t="s">
+        <v>318</v>
+      </c>
+      <c r="I15" t="s">
         <v>319</v>
-      </c>
-      <c r="I15" t="s">
-        <v>320</v>
       </c>
       <c r="J15">
         <v>47.47</v>
@@ -4583,10 +4578,10 @@
         <v>7.5</v>
       </c>
       <c r="L15" t="s">
+        <v>320</v>
+      </c>
+      <c r="M15" t="s">
         <v>321</v>
-      </c>
-      <c r="M15" t="s">
-        <v>322</v>
       </c>
       <c r="N15">
         <v>2014</v>
@@ -4597,7 +4592,7 @@
       <c r="P15" t="s">
         <v>299</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="18">
         <v>42099</v>
       </c>
       <c r="S15" t="s">
@@ -4613,7 +4608,7 @@
         <v>304</v>
       </c>
       <c r="Y15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA15">
         <v>190.72200000000001</v>
@@ -4622,16 +4617,16 @@
         <v>5</v>
       </c>
       <c r="AC15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD15">
         <v>22</v>
       </c>
       <c r="AE15" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>212</v>
       </c>
@@ -4639,22 +4634,22 @@
         <v>303</v>
       </c>
       <c r="C16" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" t="s">
         <v>312</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>313</v>
       </c>
-      <c r="E16" t="s">
-        <v>314</v>
-      </c>
       <c r="G16" t="s">
         <v>299</v>
       </c>
       <c r="H16" t="s">
+        <v>318</v>
+      </c>
+      <c r="I16" t="s">
         <v>319</v>
-      </c>
-      <c r="I16" t="s">
-        <v>320</v>
       </c>
       <c r="J16">
         <v>47.47</v>
@@ -4663,10 +4658,10 @@
         <v>7.5</v>
       </c>
       <c r="L16" t="s">
+        <v>320</v>
+      </c>
+      <c r="M16" t="s">
         <v>321</v>
-      </c>
-      <c r="M16" t="s">
-        <v>322</v>
       </c>
       <c r="N16">
         <v>2014</v>
@@ -4677,7 +4672,7 @@
       <c r="P16" t="s">
         <v>299</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="Q16" s="18">
         <v>41760</v>
       </c>
       <c r="S16" t="s">
@@ -4693,7 +4688,7 @@
         <v>304</v>
       </c>
       <c r="Y16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA16">
         <v>50.515000000000001</v>
@@ -4702,16 +4697,16 @@
         <v>5</v>
       </c>
       <c r="AC16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD16">
         <v>24</v>
       </c>
       <c r="AE16" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>212</v>
       </c>
@@ -4719,22 +4714,22 @@
         <v>303</v>
       </c>
       <c r="C17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" t="s">
         <v>312</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>313</v>
       </c>
-      <c r="E17" t="s">
-        <v>314</v>
-      </c>
       <c r="G17" t="s">
         <v>299</v>
       </c>
       <c r="H17" t="s">
+        <v>318</v>
+      </c>
+      <c r="I17" t="s">
         <v>319</v>
-      </c>
-      <c r="I17" t="s">
-        <v>320</v>
       </c>
       <c r="J17">
         <v>47.47</v>
@@ -4743,10 +4738,10 @@
         <v>7.5</v>
       </c>
       <c r="L17" t="s">
+        <v>320</v>
+      </c>
+      <c r="M17" t="s">
         <v>321</v>
-      </c>
-      <c r="M17" t="s">
-        <v>322</v>
       </c>
       <c r="N17">
         <v>2014</v>
@@ -4757,7 +4752,7 @@
       <c r="P17" t="s">
         <v>299</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="18">
         <v>41776</v>
       </c>
       <c r="S17" t="s">
@@ -4773,7 +4768,7 @@
         <v>304</v>
       </c>
       <c r="Y17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA17">
         <v>0</v>
@@ -4782,13 +4777,13 @@
         <v>5</v>
       </c>
       <c r="AC17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE17" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>212</v>
       </c>
@@ -4796,22 +4791,22 @@
         <v>303</v>
       </c>
       <c r="C18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D18" t="s">
         <v>312</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>313</v>
       </c>
-      <c r="E18" t="s">
-        <v>314</v>
-      </c>
       <c r="G18" t="s">
         <v>299</v>
       </c>
       <c r="H18" t="s">
+        <v>318</v>
+      </c>
+      <c r="I18" t="s">
         <v>319</v>
-      </c>
-      <c r="I18" t="s">
-        <v>320</v>
       </c>
       <c r="J18">
         <v>47.47</v>
@@ -4820,10 +4815,10 @@
         <v>7.5</v>
       </c>
       <c r="L18" t="s">
+        <v>320</v>
+      </c>
+      <c r="M18" t="s">
         <v>321</v>
-      </c>
-      <c r="M18" t="s">
-        <v>322</v>
       </c>
       <c r="N18">
         <v>2014</v>
@@ -4834,7 +4829,7 @@
       <c r="P18" t="s">
         <v>299</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="18">
         <v>41789</v>
       </c>
       <c r="S18" t="s">
@@ -4850,7 +4845,7 @@
         <v>304</v>
       </c>
       <c r="Y18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA18">
         <v>0</v>
@@ -4859,13 +4854,13 @@
         <v>5</v>
       </c>
       <c r="AC18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE18" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>212</v>
       </c>
@@ -4873,22 +4868,22 @@
         <v>303</v>
       </c>
       <c r="C19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D19" t="s">
+        <v>314</v>
+      </c>
+      <c r="E19" t="s">
         <v>315</v>
       </c>
-      <c r="E19" t="s">
-        <v>316</v>
-      </c>
       <c r="G19" t="s">
         <v>299</v>
       </c>
       <c r="H19" t="s">
+        <v>318</v>
+      </c>
+      <c r="I19" t="s">
         <v>319</v>
-      </c>
-      <c r="I19" t="s">
-        <v>320</v>
       </c>
       <c r="J19">
         <v>47.47</v>
@@ -4897,10 +4892,10 @@
         <v>7.5</v>
       </c>
       <c r="L19" t="s">
+        <v>320</v>
+      </c>
+      <c r="M19" t="s">
         <v>321</v>
-      </c>
-      <c r="M19" t="s">
-        <v>322</v>
       </c>
       <c r="N19">
         <v>2014</v>
@@ -4911,7 +4906,7 @@
       <c r="P19" t="s">
         <v>299</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="18">
         <v>41668</v>
       </c>
       <c r="S19" t="s">
@@ -4927,7 +4922,7 @@
         <v>304</v>
       </c>
       <c r="Y19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA19">
         <v>243.077</v>
@@ -4936,16 +4931,16 @@
         <v>5</v>
       </c>
       <c r="AC19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD19">
         <v>26</v>
       </c>
       <c r="AE19" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>212</v>
       </c>
@@ -4953,22 +4948,22 @@
         <v>303</v>
       </c>
       <c r="C20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D20" t="s">
+        <v>314</v>
+      </c>
+      <c r="E20" t="s">
         <v>315</v>
       </c>
-      <c r="E20" t="s">
-        <v>316</v>
-      </c>
       <c r="G20" t="s">
         <v>299</v>
       </c>
       <c r="H20" t="s">
+        <v>318</v>
+      </c>
+      <c r="I20" t="s">
         <v>319</v>
-      </c>
-      <c r="I20" t="s">
-        <v>320</v>
       </c>
       <c r="J20">
         <v>47.47</v>
@@ -4977,10 +4972,10 @@
         <v>7.5</v>
       </c>
       <c r="L20" t="s">
+        <v>320</v>
+      </c>
+      <c r="M20" t="s">
         <v>321</v>
-      </c>
-      <c r="M20" t="s">
-        <v>322</v>
       </c>
       <c r="N20">
         <v>2014</v>
@@ -4991,7 +4986,7 @@
       <c r="P20" t="s">
         <v>299</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q20" s="18">
         <v>41697</v>
       </c>
       <c r="S20" t="s">
@@ -5007,7 +5002,7 @@
         <v>304</v>
       </c>
       <c r="Y20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA20">
         <v>126.154</v>
@@ -5016,16 +5011,16 @@
         <v>5</v>
       </c>
       <c r="AC20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD20">
         <v>26</v>
       </c>
       <c r="AE20" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>212</v>
       </c>
@@ -5033,22 +5028,22 @@
         <v>303</v>
       </c>
       <c r="C21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D21" t="s">
+        <v>314</v>
+      </c>
+      <c r="E21" t="s">
         <v>315</v>
       </c>
-      <c r="E21" t="s">
-        <v>316</v>
-      </c>
       <c r="G21" t="s">
         <v>299</v>
       </c>
       <c r="H21" t="s">
+        <v>318</v>
+      </c>
+      <c r="I21" t="s">
         <v>319</v>
-      </c>
-      <c r="I21" t="s">
-        <v>320</v>
       </c>
       <c r="J21">
         <v>47.47</v>
@@ -5057,10 +5052,10 @@
         <v>7.5</v>
       </c>
       <c r="L21" t="s">
+        <v>320</v>
+      </c>
+      <c r="M21" t="s">
         <v>321</v>
-      </c>
-      <c r="M21" t="s">
-        <v>322</v>
       </c>
       <c r="N21">
         <v>2014</v>
@@ -5071,7 +5066,7 @@
       <c r="P21" t="s">
         <v>299</v>
       </c>
-      <c r="Q21" s="21">
+      <c r="Q21" s="18">
         <v>42099</v>
       </c>
       <c r="S21" t="s">
@@ -5087,7 +5082,7 @@
         <v>304</v>
       </c>
       <c r="Y21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA21">
         <v>0</v>
@@ -5096,13 +5091,13 @@
         <v>5</v>
       </c>
       <c r="AC21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE21" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>212</v>
       </c>
@@ -5110,22 +5105,22 @@
         <v>303</v>
       </c>
       <c r="C22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D22" t="s">
+        <v>314</v>
+      </c>
+      <c r="E22" t="s">
         <v>315</v>
       </c>
-      <c r="E22" t="s">
-        <v>316</v>
-      </c>
       <c r="G22" t="s">
         <v>299</v>
       </c>
       <c r="H22" t="s">
+        <v>318</v>
+      </c>
+      <c r="I22" t="s">
         <v>319</v>
-      </c>
-      <c r="I22" t="s">
-        <v>320</v>
       </c>
       <c r="J22">
         <v>47.47</v>
@@ -5134,10 +5129,10 @@
         <v>7.5</v>
       </c>
       <c r="L22" t="s">
+        <v>320</v>
+      </c>
+      <c r="M22" t="s">
         <v>321</v>
-      </c>
-      <c r="M22" t="s">
-        <v>322</v>
       </c>
       <c r="N22">
         <v>2014</v>
@@ -5148,7 +5143,7 @@
       <c r="P22" t="s">
         <v>299</v>
       </c>
-      <c r="Q22" s="21">
+      <c r="Q22" s="18">
         <v>41760</v>
       </c>
       <c r="S22" t="s">
@@ -5164,7 +5159,7 @@
         <v>304</v>
       </c>
       <c r="Y22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA22">
         <v>0</v>
@@ -5173,13 +5168,13 @@
         <v>5</v>
       </c>
       <c r="AC22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE22" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>212</v>
       </c>
@@ -5187,22 +5182,22 @@
         <v>303</v>
       </c>
       <c r="C23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D23" t="s">
+        <v>314</v>
+      </c>
+      <c r="E23" t="s">
         <v>315</v>
       </c>
-      <c r="E23" t="s">
-        <v>316</v>
-      </c>
       <c r="G23" t="s">
         <v>299</v>
       </c>
       <c r="H23" t="s">
+        <v>318</v>
+      </c>
+      <c r="I23" t="s">
         <v>319</v>
-      </c>
-      <c r="I23" t="s">
-        <v>320</v>
       </c>
       <c r="J23">
         <v>47.47</v>
@@ -5211,10 +5206,10 @@
         <v>7.5</v>
       </c>
       <c r="L23" t="s">
+        <v>320</v>
+      </c>
+      <c r="M23" t="s">
         <v>321</v>
-      </c>
-      <c r="M23" t="s">
-        <v>322</v>
       </c>
       <c r="N23">
         <v>2014</v>
@@ -5225,7 +5220,7 @@
       <c r="P23" t="s">
         <v>299</v>
       </c>
-      <c r="Q23" s="21">
+      <c r="Q23" s="18">
         <v>41776</v>
       </c>
       <c r="S23" t="s">
@@ -5241,7 +5236,7 @@
         <v>304</v>
       </c>
       <c r="Y23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -5250,13 +5245,13 @@
         <v>5</v>
       </c>
       <c r="AC23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE23" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>212</v>
       </c>
@@ -5264,22 +5259,22 @@
         <v>303</v>
       </c>
       <c r="C24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D24" t="s">
+        <v>316</v>
+      </c>
+      <c r="E24" t="s">
         <v>317</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
+        <v>299</v>
+      </c>
+      <c r="H24" t="s">
         <v>318</v>
       </c>
-      <c r="G24" t="s">
-        <v>299</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>319</v>
-      </c>
-      <c r="I24" t="s">
-        <v>320</v>
       </c>
       <c r="J24">
         <v>47.47</v>
@@ -5288,10 +5283,10 @@
         <v>7.5</v>
       </c>
       <c r="L24" t="s">
+        <v>320</v>
+      </c>
+      <c r="M24" t="s">
         <v>321</v>
-      </c>
-      <c r="M24" t="s">
-        <v>322</v>
       </c>
       <c r="N24">
         <v>2014</v>
@@ -5302,7 +5297,7 @@
       <c r="P24" t="s">
         <v>299</v>
       </c>
-      <c r="Q24" s="21">
+      <c r="Q24" s="18">
         <v>41668</v>
       </c>
       <c r="S24" t="s">
@@ -5318,7 +5313,7 @@
         <v>304</v>
       </c>
       <c r="Y24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA24">
         <v>390.74599999999998</v>
@@ -5327,13 +5322,13 @@
         <v>5</v>
       </c>
       <c r="AC24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE24" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>212</v>
       </c>
@@ -5341,22 +5336,22 @@
         <v>303</v>
       </c>
       <c r="C25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D25" t="s">
+        <v>316</v>
+      </c>
+      <c r="E25" t="s">
         <v>317</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
+        <v>299</v>
+      </c>
+      <c r="H25" t="s">
         <v>318</v>
       </c>
-      <c r="G25" t="s">
-        <v>299</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>319</v>
-      </c>
-      <c r="I25" t="s">
-        <v>320</v>
       </c>
       <c r="J25">
         <v>47.47</v>
@@ -5365,10 +5360,10 @@
         <v>7.5</v>
       </c>
       <c r="L25" t="s">
+        <v>320</v>
+      </c>
+      <c r="M25" t="s">
         <v>321</v>
-      </c>
-      <c r="M25" t="s">
-        <v>322</v>
       </c>
       <c r="N25">
         <v>2014</v>
@@ -5379,7 +5374,7 @@
       <c r="P25" t="s">
         <v>299</v>
       </c>
-      <c r="Q25" s="21">
+      <c r="Q25" s="18">
         <v>41697</v>
       </c>
       <c r="S25" t="s">
@@ -5395,7 +5390,7 @@
         <v>304</v>
       </c>
       <c r="Y25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA25">
         <v>332.13400000000001</v>
@@ -5404,13 +5399,13 @@
         <v>5</v>
       </c>
       <c r="AC25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE25" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -5418,22 +5413,22 @@
         <v>303</v>
       </c>
       <c r="C26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E26" t="s">
         <v>317</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
+        <v>299</v>
+      </c>
+      <c r="H26" t="s">
         <v>318</v>
       </c>
-      <c r="G26" t="s">
-        <v>299</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>319</v>
-      </c>
-      <c r="I26" t="s">
-        <v>320</v>
       </c>
       <c r="J26">
         <v>47.47</v>
@@ -5442,10 +5437,10 @@
         <v>7.5</v>
       </c>
       <c r="L26" t="s">
+        <v>320</v>
+      </c>
+      <c r="M26" t="s">
         <v>321</v>
-      </c>
-      <c r="M26" t="s">
-        <v>322</v>
       </c>
       <c r="N26">
         <v>2014</v>
@@ -5456,7 +5451,7 @@
       <c r="P26" t="s">
         <v>299</v>
       </c>
-      <c r="Q26" s="21">
+      <c r="Q26" s="18">
         <v>42099</v>
       </c>
       <c r="S26" t="s">
@@ -5472,7 +5467,7 @@
         <v>304</v>
       </c>
       <c r="Y26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA26">
         <v>177.892</v>
@@ -5481,13 +5476,13 @@
         <v>5</v>
       </c>
       <c r="AC26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE26" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>212</v>
       </c>
@@ -5495,22 +5490,22 @@
         <v>303</v>
       </c>
       <c r="C27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D27" t="s">
+        <v>316</v>
+      </c>
+      <c r="E27" t="s">
         <v>317</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
+        <v>299</v>
+      </c>
+      <c r="H27" t="s">
         <v>318</v>
       </c>
-      <c r="G27" t="s">
-        <v>299</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>319</v>
-      </c>
-      <c r="I27" t="s">
-        <v>320</v>
       </c>
       <c r="J27">
         <v>47.47</v>
@@ -5519,10 +5514,10 @@
         <v>7.5</v>
       </c>
       <c r="L27" t="s">
+        <v>320</v>
+      </c>
+      <c r="M27" t="s">
         <v>321</v>
-      </c>
-      <c r="M27" t="s">
-        <v>322</v>
       </c>
       <c r="N27">
         <v>2014</v>
@@ -5533,7 +5528,7 @@
       <c r="P27" t="s">
         <v>299</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="18">
         <v>41760</v>
       </c>
       <c r="S27" t="s">
@@ -5549,7 +5544,7 @@
         <v>304</v>
       </c>
       <c r="Y27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA27">
         <v>47.301000000000002</v>
@@ -5558,13 +5553,13 @@
         <v>5</v>
       </c>
       <c r="AC27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE27" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>212</v>
       </c>
@@ -5572,22 +5567,22 @@
         <v>303</v>
       </c>
       <c r="C28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D28" t="s">
+        <v>316</v>
+      </c>
+      <c r="E28" t="s">
         <v>317</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
+        <v>299</v>
+      </c>
+      <c r="H28" t="s">
         <v>318</v>
       </c>
-      <c r="G28" t="s">
-        <v>299</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>319</v>
-      </c>
-      <c r="I28" t="s">
-        <v>320</v>
       </c>
       <c r="J28">
         <v>47.47</v>
@@ -5596,10 +5591,10 @@
         <v>7.5</v>
       </c>
       <c r="L28" t="s">
+        <v>320</v>
+      </c>
+      <c r="M28" t="s">
         <v>321</v>
-      </c>
-      <c r="M28" t="s">
-        <v>322</v>
       </c>
       <c r="N28">
         <v>2014</v>
@@ -5610,7 +5605,7 @@
       <c r="P28" t="s">
         <v>299</v>
       </c>
-      <c r="Q28" s="21">
+      <c r="Q28" s="18">
         <v>41776</v>
       </c>
       <c r="S28" t="s">
@@ -5626,7 +5621,7 @@
         <v>304</v>
       </c>
       <c r="Y28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA28">
         <v>0</v>
@@ -5635,13 +5630,13 @@
         <v>5</v>
       </c>
       <c r="AC28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE28" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>212</v>
       </c>
@@ -5649,22 +5644,22 @@
         <v>303</v>
       </c>
       <c r="C29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D29" t="s">
+        <v>316</v>
+      </c>
+      <c r="E29" t="s">
         <v>317</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
+        <v>299</v>
+      </c>
+      <c r="H29" t="s">
         <v>318</v>
       </c>
-      <c r="G29" t="s">
-        <v>299</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>319</v>
-      </c>
-      <c r="I29" t="s">
-        <v>320</v>
       </c>
       <c r="J29">
         <v>47.47</v>
@@ -5673,10 +5668,10 @@
         <v>7.5</v>
       </c>
       <c r="L29" t="s">
+        <v>320</v>
+      </c>
+      <c r="M29" t="s">
         <v>321</v>
-      </c>
-      <c r="M29" t="s">
-        <v>322</v>
       </c>
       <c r="N29">
         <v>2014</v>
@@ -5687,7 +5682,7 @@
       <c r="P29" t="s">
         <v>299</v>
       </c>
-      <c r="Q29" s="21">
+      <c r="Q29" s="18">
         <v>41789</v>
       </c>
       <c r="S29" t="s">
@@ -5703,7 +5698,7 @@
         <v>304</v>
       </c>
       <c r="Y29" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -5712,13 +5707,13 @@
         <v>5</v>
       </c>
       <c r="AC29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE29" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>212</v>
       </c>
@@ -5726,22 +5721,22 @@
         <v>303</v>
       </c>
       <c r="C30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D30" t="s">
+        <v>322</v>
+      </c>
+      <c r="E30" t="s">
         <v>323</v>
       </c>
-      <c r="E30" t="s">
-        <v>324</v>
-      </c>
       <c r="G30" t="s">
         <v>299</v>
       </c>
       <c r="H30" t="s">
+        <v>318</v>
+      </c>
+      <c r="I30" t="s">
         <v>319</v>
-      </c>
-      <c r="I30" t="s">
-        <v>320</v>
       </c>
       <c r="J30">
         <v>47.47</v>
@@ -5750,10 +5745,10 @@
         <v>7.5</v>
       </c>
       <c r="L30" t="s">
+        <v>320</v>
+      </c>
+      <c r="M30" t="s">
         <v>321</v>
-      </c>
-      <c r="M30" t="s">
-        <v>322</v>
       </c>
       <c r="N30">
         <v>2014</v>
@@ -5764,7 +5759,7 @@
       <c r="P30" t="s">
         <v>299</v>
       </c>
-      <c r="Q30" s="21">
+      <c r="Q30" s="18">
         <v>41668</v>
       </c>
       <c r="S30" t="s">
@@ -5780,7 +5775,7 @@
         <v>304</v>
       </c>
       <c r="Y30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA30">
         <v>321.851</v>
@@ -5789,16 +5784,16 @@
         <v>4</v>
       </c>
       <c r="AC30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD30">
         <v>33</v>
       </c>
       <c r="AE30" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>212</v>
       </c>
@@ -5806,22 +5801,22 @@
         <v>303</v>
       </c>
       <c r="C31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D31" t="s">
+        <v>322</v>
+      </c>
+      <c r="E31" t="s">
         <v>323</v>
       </c>
-      <c r="E31" t="s">
-        <v>324</v>
-      </c>
       <c r="G31" t="s">
         <v>299</v>
       </c>
       <c r="H31" t="s">
+        <v>318</v>
+      </c>
+      <c r="I31" t="s">
         <v>319</v>
-      </c>
-      <c r="I31" t="s">
-        <v>320</v>
       </c>
       <c r="J31">
         <v>47.47</v>
@@ -5830,10 +5825,10 @@
         <v>7.5</v>
       </c>
       <c r="L31" t="s">
+        <v>320</v>
+      </c>
+      <c r="M31" t="s">
         <v>321</v>
-      </c>
-      <c r="M31" t="s">
-        <v>322</v>
       </c>
       <c r="N31">
         <v>2014</v>
@@ -5844,7 +5839,7 @@
       <c r="P31" t="s">
         <v>299</v>
       </c>
-      <c r="Q31" s="21">
+      <c r="Q31" s="18">
         <v>41697</v>
       </c>
       <c r="S31" t="s">
@@ -5860,7 +5855,7 @@
         <v>304</v>
       </c>
       <c r="Y31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA31">
         <v>183.03299999999999</v>
@@ -5869,16 +5864,16 @@
         <v>4</v>
       </c>
       <c r="AC31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD31">
         <v>30</v>
       </c>
       <c r="AE31" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>212</v>
       </c>
@@ -5886,22 +5881,22 @@
         <v>303</v>
       </c>
       <c r="C32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E32" t="s">
         <v>323</v>
       </c>
-      <c r="E32" t="s">
-        <v>324</v>
-      </c>
       <c r="G32" t="s">
         <v>299</v>
       </c>
       <c r="H32" t="s">
+        <v>318</v>
+      </c>
+      <c r="I32" t="s">
         <v>319</v>
-      </c>
-      <c r="I32" t="s">
-        <v>320</v>
       </c>
       <c r="J32">
         <v>47.47</v>
@@ -5910,10 +5905,10 @@
         <v>7.5</v>
       </c>
       <c r="L32" t="s">
+        <v>320</v>
+      </c>
+      <c r="M32" t="s">
         <v>321</v>
-      </c>
-      <c r="M32" t="s">
-        <v>322</v>
       </c>
       <c r="N32">
         <v>2014</v>
@@ -5924,7 +5919,7 @@
       <c r="P32" t="s">
         <v>299</v>
       </c>
-      <c r="Q32" s="21">
+      <c r="Q32" s="18">
         <v>42099</v>
       </c>
       <c r="S32" t="s">
@@ -5940,7 +5935,7 @@
         <v>304</v>
       </c>
       <c r="Y32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA32">
         <v>58.612000000000002</v>
@@ -5949,16 +5944,16 @@
         <v>4</v>
       </c>
       <c r="AC32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD32">
         <v>32</v>
       </c>
       <c r="AE32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>212</v>
       </c>
@@ -5966,22 +5961,22 @@
         <v>303</v>
       </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D33" t="s">
+        <v>322</v>
+      </c>
+      <c r="E33" t="s">
         <v>323</v>
       </c>
-      <c r="E33" t="s">
-        <v>324</v>
-      </c>
       <c r="G33" t="s">
         <v>299</v>
       </c>
       <c r="H33" t="s">
+        <v>318</v>
+      </c>
+      <c r="I33" t="s">
         <v>319</v>
-      </c>
-      <c r="I33" t="s">
-        <v>320</v>
       </c>
       <c r="J33">
         <v>47.47</v>
@@ -5990,10 +5985,10 @@
         <v>7.5</v>
       </c>
       <c r="L33" t="s">
+        <v>320</v>
+      </c>
+      <c r="M33" t="s">
         <v>321</v>
-      </c>
-      <c r="M33" t="s">
-        <v>322</v>
       </c>
       <c r="N33">
         <v>2014</v>
@@ -6004,7 +5999,7 @@
       <c r="P33" t="s">
         <v>299</v>
       </c>
-      <c r="Q33" s="21">
+      <c r="Q33" s="18">
         <v>41760</v>
       </c>
       <c r="S33" t="s">
@@ -6020,7 +6015,7 @@
         <v>304</v>
       </c>
       <c r="Y33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA33">
         <v>0</v>
@@ -6029,13 +6024,13 @@
         <v>4</v>
       </c>
       <c r="AC33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE33" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>212</v>
       </c>
@@ -6043,22 +6038,22 @@
         <v>303</v>
       </c>
       <c r="C34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D34" t="s">
+        <v>322</v>
+      </c>
+      <c r="E34" t="s">
         <v>323</v>
       </c>
-      <c r="E34" t="s">
-        <v>324</v>
-      </c>
       <c r="G34" t="s">
         <v>299</v>
       </c>
       <c r="H34" t="s">
+        <v>318</v>
+      </c>
+      <c r="I34" t="s">
         <v>319</v>
-      </c>
-      <c r="I34" t="s">
-        <v>320</v>
       </c>
       <c r="J34">
         <v>47.47</v>
@@ -6067,10 +6062,10 @@
         <v>7.5</v>
       </c>
       <c r="L34" t="s">
+        <v>320</v>
+      </c>
+      <c r="M34" t="s">
         <v>321</v>
-      </c>
-      <c r="M34" t="s">
-        <v>322</v>
       </c>
       <c r="N34">
         <v>2014</v>
@@ -6081,7 +6076,7 @@
       <c r="P34" t="s">
         <v>299</v>
       </c>
-      <c r="Q34" s="21">
+      <c r="Q34" s="18">
         <v>41776</v>
       </c>
       <c r="S34" t="s">
@@ -6097,22 +6092,22 @@
         <v>304</v>
       </c>
       <c r="Y34" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AB34">
         <v>4</v>
       </c>
       <c r="AC34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE34" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>212</v>
       </c>
@@ -6120,22 +6115,22 @@
         <v>303</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D35" t="s">
+        <v>322</v>
+      </c>
+      <c r="E35" t="s">
         <v>323</v>
       </c>
-      <c r="E35" t="s">
-        <v>324</v>
-      </c>
       <c r="G35" t="s">
         <v>299</v>
       </c>
       <c r="H35" t="s">
+        <v>318</v>
+      </c>
+      <c r="I35" t="s">
         <v>319</v>
-      </c>
-      <c r="I35" t="s">
-        <v>320</v>
       </c>
       <c r="J35">
         <v>47.47</v>
@@ -6144,10 +6139,10 @@
         <v>7.5</v>
       </c>
       <c r="L35" t="s">
+        <v>320</v>
+      </c>
+      <c r="M35" t="s">
         <v>321</v>
-      </c>
-      <c r="M35" t="s">
-        <v>322</v>
       </c>
       <c r="N35">
         <v>2014</v>
@@ -6158,7 +6153,7 @@
       <c r="P35" t="s">
         <v>299</v>
       </c>
-      <c r="Q35" s="21">
+      <c r="Q35" s="18">
         <v>41789</v>
       </c>
       <c r="S35" t="s">
@@ -6174,19 +6169,19 @@
         <v>304</v>
       </c>
       <c r="Y35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA35" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AB35">
         <v>4</v>
       </c>
       <c r="AC35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -6209,14 +6204,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>281</v>
       </c>

</xml_diff>